<commit_message>
updated repo for case study
</commit_message>
<xml_diff>
--- a/src/data/demo_dataset.xlsx
+++ b/src/data/demo_dataset.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/aiswre/src/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_7C3981EFF613C8064815742E78963A1E6D185641" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05BDB09B-7413-414D-9200-30A069C386FA}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Requirement_#</t>
-  </si>
-  <si>
-    <t>Requirement</t>
-  </si>
-  <si>
     <t>The Disputes System shall record the name of the user and the date for any activity that creates or modifies the disputes case in the system.  A detailed history of the actions taken on the case  including the date and the user that performed the action must be maintained for auditing purposes.</t>
   </si>
   <si>
@@ -35,13 +35,19 @@
   </si>
   <si>
     <t>The product shall be platform independent.The product shall enable access to any type of development environment and platform.</t>
+  </si>
+  <si>
+    <t>requirement</t>
+  </si>
+  <si>
+    <t>requirement_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,13 +110,25 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -148,7 +166,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -182,6 +200,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -216,9 +235,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -391,22 +411,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="112.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -414,10 +439,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -425,10 +450,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -436,10 +461,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -447,10 +472,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -458,7 +483,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated prompt processor to parse json more robustly as it is returned from llm
</commit_message>
<xml_diff>
--- a/src/data/demo_dataset.xlsx
+++ b/src/data/demo_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/aiswre/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_7C3981EFF613C8064815742E78963A1E6D185641" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05BDB09B-7413-414D-9200-30A069C386FA}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_7C3981EFF613C8064815742E78963A1E6D185641" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9AF9FC5-6AFB-42A6-8325-7586D2737831}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,10 +37,10 @@
     <t>The product shall be platform independent.The product shall enable access to any type of development environment and platform.</t>
   </si>
   <si>
-    <t>requirement</t>
-  </si>
-  <si>
     <t>requirement_id</t>
+  </si>
+  <si>
+    <t>requirements</t>
   </si>
 </sst>
 </file>
@@ -119,10 +119,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,7 +411,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -425,10 +421,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>